<commit_message>
combined model into merge
</commit_message>
<xml_diff>
--- a/merge/results/comparison_results.xlsx
+++ b/merge/results/comparison_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haddo\DL_stack\Halimeda\combined_model\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haddo\DL_stack\Halimeda\merge\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4230EB64-37E2-4E6F-A87D-CF4E63652977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91724C4E-1FF8-45D7-A8F0-6F725F4D0EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C741A474-2E85-4CAE-8F7D-A785337B78F1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>1024_3_000033_c</t>
   </si>
@@ -117,9 +117,6 @@
     <t>combined_weights</t>
   </si>
   <si>
-    <t>Combined model 0</t>
-  </si>
-  <si>
     <t>all_test</t>
   </si>
   <si>
@@ -127,13 +124,23 @@
   </si>
   <si>
     <t>SS best run k fold test (fold c )</t>
+  </si>
+  <si>
+    <t>Combinded model W  (0.8OD+0.2SS)</t>
+  </si>
+  <si>
+    <t>Combined model W (0.5-0.5)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,8 +178,15 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +268,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,10 +302,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -367,9 +388,14 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -686,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C125F3D0-A53A-45E7-8347-62C18A50907B}">
-  <dimension ref="A4:O19"/>
+  <dimension ref="A4:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +763,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>0</v>
@@ -809,7 +835,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="15">
         <v>96</v>
@@ -866,7 +892,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>26</v>
@@ -895,7 +921,34 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J10" s="10"/>
+      <c r="A10" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="26">
+        <v>22</v>
+      </c>
+      <c r="D10" s="26">
+        <v>0.90939863840738933</v>
+      </c>
+      <c r="E10" s="26">
+        <v>0.84080452102829617</v>
+      </c>
+      <c r="F10" s="26">
+        <v>0.91281748753302627</v>
+      </c>
+      <c r="G10" s="26">
+        <v>9.2429765512481096E-2</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0.87533238821645398</v>
+      </c>
+      <c r="I10" s="26">
+        <v>0.96001247703654569</v>
+      </c>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J11" s="10"/>
@@ -905,7 +958,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1078,6 +1131,32 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="B20" s="29">
+        <v>22</v>
+      </c>
+      <c r="C20" s="32">
+        <v>0.90939863840738933</v>
+      </c>
+      <c r="D20" s="32">
+        <v>0.84080452102829617</v>
+      </c>
+      <c r="E20" s="30">
+        <v>0.91281748753302627</v>
+      </c>
+      <c r="F20" s="30">
+        <v>9.2429765512481096E-2</v>
+      </c>
+      <c r="G20" s="31">
+        <v>0.87533238821645432</v>
+      </c>
+      <c r="H20" s="30">
+        <v>0.96001247703654569</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>